<commit_message>
added transactionID to Async IEPD
added transactionID to Async IEPD
</commit_message>
<xml_diff>
--- a/schemas/AsyncResponse_iepd/artifacts/Async_Response_MappingSpreadsheet.xlsx
+++ b/schemas/AsyncResponse_iepd/artifacts/Async_Response_MappingSpreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcp911gov-my.sharepoint.com/personal/aidandelgado_missioncriticalpartners_com/Documents/ONE.WORKSPACE/21. NOLA/EXCHANGES/ASYNC BOOKING/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcp911gov-my.sharepoint.com/personal/aidandelgado_missioncriticalpartners_com/Documents/ONE.WORKSPACE/21. NOLA/EXCHANGES/ASYNC BOOKING/AsyncResponse_iepd/artifacts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D18CB6CD-8FD1-4883-847E-53F87FC2A679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="158" documentId="11_B43F5A2CC41A4E1DE1EE3DC0A71BBEAA7677294A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8236E933-7693-4AF5-962D-0B5776637B16}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-4170" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-4575" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Async Response" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="101">
   <si>
     <t>ID</t>
   </si>
@@ -62,6 +62,15 @@
     <t>3</t>
   </si>
   <si>
+    <t>NOLAObjectType</t>
+  </si>
+  <si>
+    <t>An object type for the different data exchanges involded in the NOLA JTMP Azure Enterprise service Bus (ESB).</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
     <t>ProcessingErrorDetails</t>
   </si>
   <si>
@@ -71,7 +80,7 @@
     <t>Attribute</t>
   </si>
   <si>
-    <t>5</t>
+    <t>7</t>
   </si>
   <si>
     <t>errorCodeText</t>
@@ -83,7 +92,7 @@
     <t>A text value for an error code that occurred during the processing of a message.</t>
   </si>
   <si>
-    <t>6</t>
+    <t>8</t>
   </si>
   <si>
     <t>errorDescriptionText</t>
@@ -92,7 +101,7 @@
     <t>A text description of the error details.</t>
   </si>
   <si>
-    <t>7</t>
+    <t>9</t>
   </si>
   <si>
     <t>ContentErrorDetails</t>
@@ -101,22 +110,22 @@
     <t>An XML related error with the payload of a message that was sent. This is most likely going to be related to business rules errors that XML schema validation does not encounter.</t>
   </si>
   <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
     <t>11</t>
   </si>
   <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
     <t>AsynchronousResponse</t>
   </si>
   <si>
     <t>An asynchronous response of an XML transaction between two API endpoints.</t>
   </si>
   <si>
-    <t>13</t>
+    <t>15</t>
   </si>
   <si>
     <t>responseDateTime</t>
@@ -128,7 +137,7 @@
     <t>A date and time the response was received.</t>
   </si>
   <si>
-    <t>14</t>
+    <t>16</t>
   </si>
   <si>
     <t>transactionStatusCode</t>
@@ -137,7 +146,7 @@
     <t>A code specifying the status of the transaction.</t>
   </si>
   <si>
-    <t>15</t>
+    <t>17</t>
   </si>
   <si>
     <t>responseDescription</t>
@@ -149,16 +158,25 @@
     <t>0..1</t>
   </si>
   <si>
-    <t>16</t>
+    <t>18</t>
   </si>
   <si>
     <t>transactionID</t>
   </si>
   <si>
+    <t>The original transactionID that was set by the originator of the message.</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>messageID</t>
+  </si>
+  <si>
     <t>A unique string identifier that preserves the identity of the exchange transaction end to end, which facilitates the correlation of asynchronous response messages to their original request.</t>
   </si>
   <si>
-    <t>17</t>
+    <t>20</t>
   </si>
   <si>
     <t>destinationAgency</t>
@@ -167,7 +185,7 @@
     <t>The destination agency to whom the request was related to. This is not required but is a middleware debugging convenience.</t>
   </si>
   <si>
-    <t>18</t>
+    <t>21</t>
   </si>
   <si>
     <t>contextualResponseMessage</t>
@@ -179,7 +197,7 @@
     <t>Association</t>
   </si>
   <si>
-    <t>19</t>
+    <t>22</t>
   </si>
   <si>
     <t>SchemaError</t>
@@ -188,19 +206,10 @@
     <t>0..*</t>
   </si>
   <si>
-    <t>22</t>
+    <t>25</t>
   </si>
   <si>
     <t>ProcessingError</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>NOLAObjectType</t>
-  </si>
-  <si>
-    <t>An object type for the different data exchanges involded in the NOLA JTMP Azure Enterprise service Bus (ESB).</t>
   </si>
   <si>
     <t>&lt;&lt;NOLA&gt;&gt;
@@ -219,14 +228,13 @@
 Comments</t>
   </si>
   <si>
-    <t>&lt;&lt;NOLA&gt;&gt;
-CodeList</t>
-  </si>
-  <si>
     <t>&lt;&lt;NOLA_Exchange&gt;&gt;
 Async Response</t>
   </si>
   <si>
+    <t>/nola:AsynchronousResponseMessage</t>
+  </si>
+  <si>
     <t>cbrn:MessageErrorType</t>
   </si>
   <si>
@@ -293,6 +301,12 @@
     <t>/nola:AsynchronousResponseMessage/MessageStatus/SystemEventDescriptionText</t>
   </si>
   <si>
+    <t>nola-ext:TransactionID</t>
+  </si>
+  <si>
+    <t>/nola:AsynchronousResponseMessage/MessageStatus/nola-ext:MessageStatusAugmentation/nola-ext:TransactionID</t>
+  </si>
+  <si>
     <t>nc:MessageID</t>
   </si>
   <si>
@@ -321,9 +335,6 @@
   </si>
   <si>
     <t>When the transactionStatusCode is 'DataError' or 'Success', there will not be any processing error in the message.</t>
-  </si>
-  <si>
-    <t>/nola:AsynchronousResponseMessage</t>
   </si>
   <si>
     <t>Property Type</t>
@@ -336,7 +347,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -354,12 +365,6 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -475,7 +480,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -519,14 +524,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="18">
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -783,6 +785,21 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -815,23 +832,6 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -1030,23 +1030,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{85A3D202-2F5B-4BFD-8795-1A004A28B5C4}" name="MappingSpreadsheet" displayName="MappingSpreadsheet" ref="A1:N17" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="17" tableBorderDxfId="18" totalsRowBorderDxfId="16">
-  <autoFilter ref="A1:N17" xr:uid="{85A3D202-2F5B-4BFD-8795-1A004A28B5C4}"/>
-  <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{FBAA23B2-FCB8-4047-85DC-0CA613CE8735}" name="Property Type" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{C806218C-83DB-487E-83E4-7BF8A6D52860}" name="ID" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{B5C582F8-F52F-4C6B-9A4F-652EC5B842F0}" name="Class" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{E0488388-0AC7-4D31-9E59-8E0161152EE0}" name="Attribute" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{E196E198-7E66-4EA5-AE33-8DC5D98C7CC0}" name="Type" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{5CF471BF-EDD8-4568-AE80-3B8D0C19F6DB}" name="Description" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{9EE95595-4AFC-4096-A28E-E6D9DECC6020}" name="Multiplicity" dataDxfId="9"/>
-    <tableColumn id="14" xr3:uid="{D641F8B8-6E7C-4A7D-95F6-D3DAAA0B3555}" name="Name" dataDxfId="8"/>
-    <tableColumn id="15" xr3:uid="{5964BCC5-D455-4A84-A8F3-39562595E662}" name="&lt;&lt;NOLA&gt;&gt;_x000a_NIEM Element" dataDxfId="7"/>
-    <tableColumn id="16" xr3:uid="{4026AA03-7E37-47E1-919A-C6415649738C}" name="&lt;&lt;NOLA&gt;&gt;_x000a_NIEM Type" dataDxfId="6"/>
-    <tableColumn id="17" xr3:uid="{F3FA6A68-6E3C-4065-9BD0-26DF1C603DA6}" name="&lt;&lt;NOLA&gt;&gt;_x000a_Parent Base Type" dataDxfId="5"/>
-    <tableColumn id="23" xr3:uid="{F6CE3EDA-1B30-4D6E-8F7E-95EAEE89D16D}" name="&lt;&lt;NOLA&gt;&gt;_x000a_Comments" dataDxfId="4"/>
-    <tableColumn id="24" xr3:uid="{7F351D8B-91A0-4BFC-AE87-B169F396742C}" name="&lt;&lt;NOLA&gt;&gt;_x000a_CodeList" dataDxfId="3"/>
-    <tableColumn id="30" xr3:uid="{6438B75E-2E5B-4A7A-A1E2-A4126A7CB2F3}" name="&lt;&lt;NOLA_Exchange&gt;&gt;_x000a_Async Response" dataDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C0EE9B48-AC50-4A5D-A031-627A21142ED8}" name="MappingSpreadsheet" displayName="MappingSpreadsheet" ref="A1:M18" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="16" tableBorderDxfId="17" totalsRowBorderDxfId="15">
+  <autoFilter ref="A1:M18" xr:uid="{C0EE9B48-AC50-4A5D-A031-627A21142ED8}"/>
+  <tableColumns count="13">
+    <tableColumn id="1" xr3:uid="{4B5C1535-2F16-4A8B-A64C-AA18082D373D}" name="Property Type" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{BB8001B4-870A-4376-82B3-1C6075334386}" name="ID" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{F07FEB13-222F-40BF-9186-4598CC83146F}" name="Class" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{5BDACC57-DE6F-4A94-9AD9-897888BC2FA7}" name="Attribute" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{42FC6734-2672-4E4A-87C1-3CE725524649}" name="Type" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{F366D14B-26CC-429C-989F-4B73FED7E388}" name="Description" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{78786635-FA58-425F-A182-F07552C0CFDD}" name="Multiplicity" dataDxfId="8"/>
+    <tableColumn id="14" xr3:uid="{322466B7-F50C-4358-BE77-7F59E705FFC8}" name="Name" dataDxfId="7"/>
+    <tableColumn id="16" xr3:uid="{DC04A0F2-1C57-4501-9AD0-7B7802568ADA}" name="&lt;&lt;NOLA&gt;&gt;_x000a_NIEM Element" dataDxfId="6"/>
+    <tableColumn id="17" xr3:uid="{9B76816F-C8C8-4799-ADF7-86CE87312268}" name="&lt;&lt;NOLA&gt;&gt;_x000a_NIEM Type" dataDxfId="5"/>
+    <tableColumn id="18" xr3:uid="{2BBC1B5F-FD8A-4B6C-ADEF-AF73917B600D}" name="&lt;&lt;NOLA&gt;&gt;_x000a_Parent Base Type" dataDxfId="4"/>
+    <tableColumn id="24" xr3:uid="{7DD96120-E354-4E58-8BCD-4C2680ABF109}" name="&lt;&lt;NOLA&gt;&gt;_x000a_Comments" dataDxfId="3"/>
+    <tableColumn id="31" xr3:uid="{FA5D24B9-18B1-4753-B252-DCCB9EFDFB1C}" name="&lt;&lt;NOLA_Exchange&gt;&gt;_x000a_Async Response" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1349,7 +1348,8 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N17"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
@@ -1367,14 +1367,12 @@
     <col min="5" max="5" width="12.88671875" customWidth="1"/>
     <col min="6" max="6" width="34.109375" customWidth="1"/>
     <col min="7" max="7" width="13.21875" customWidth="1"/>
-    <col min="8" max="8" width="18.33203125" customWidth="1"/>
     <col min="9" max="13" width="11" customWidth="1"/>
-    <col min="14" max="14" width="101.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1383,7 +1381,7 @@
         <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -1398,447 +1396,431 @@
         <v>1</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="I2" s="6"/>
       <c r="J2" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="K2" s="15" t="s">
-        <v>54</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="K2" s="6"/>
       <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6" t="s">
-        <v>74</v>
+      <c r="M2" s="6" t="s">
+        <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9" t="s">
-        <v>89</v>
+      <c r="M3" s="9" t="s">
+        <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="K4" s="9"/>
       <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9" t="s">
-        <v>87</v>
+      <c r="M4" s="9" t="s">
+        <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
-        <v>47</v>
+    <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>9</v>
+        <v>28</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>17</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" s="9"/>
+        <v>46</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>45</v>
+      </c>
       <c r="I5" s="9" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="K5" s="9"/>
-      <c r="L5" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9" t="s">
-        <v>63</v>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9" t="s">
+        <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
-        <v>11</v>
+    <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>53</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="9" t="s">
-        <v>29</v>
+      <c r="D6" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="F6" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="C7" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="J6" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>37</v>
-      </c>
       <c r="H7" s="9" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9" t="s">
-        <v>83</v>
+      <c r="M7" s="9" t="s">
+        <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
-        <v>47</v>
+    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>20</v>
+        <v>28</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>17</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="H8" s="9"/>
+        <v>39</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="I8" s="9" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="K8" s="9"/>
-      <c r="L8" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9" t="s">
-        <v>70</v>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9" t="s">
+        <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
-        <v>11</v>
+    <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>53</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="M9" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="J9" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
-        <v>11</v>
-      </c>
       <c r="B10" s="8" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>6</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="K10" s="9"/>
       <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9" t="s">
-        <v>80</v>
+      <c r="M10" s="9" t="s">
+        <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G11" s="5"/>
-      <c r="H11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4" t="s">
-        <v>70</v>
+      <c r="B12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="5"/>
+      <c r="H12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4" t="s">
+        <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="9" t="s">
+    <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="I12" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="J12" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
-        <v>11</v>
-      </c>
       <c r="B13" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>20</v>
-      </c>
       <c r="D13" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="9" t="s">
         <v>17</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>14</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>18</v>
@@ -1847,54 +1829,58 @@
         <v>6</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I13" s="9" t="s">
         <v>67</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="K13" s="9"/>
       <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9" t="s">
-        <v>72</v>
+      <c r="M13" s="9" t="s">
+        <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="G14" s="5"/>
-      <c r="H14" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4" t="s">
-        <v>94</v>
+    <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9" t="s">
+        <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>7</v>
       </c>
@@ -1905,7 +1891,7 @@
         <v>9</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="4" t="s">
@@ -1916,96 +1902,124 @@
         <v>9</v>
       </c>
       <c r="I15" s="4"/>
-      <c r="J15" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="K15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4" t="s">
-        <v>63</v>
+      <c r="M15" s="4" t="s">
+        <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
+    <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="C16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="F16" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="G16" s="5"/>
+      <c r="H16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="B17" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="C17" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H16" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="I16" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="J16" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9" t="s">
-        <v>66</v>
+      <c r="H17" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9" t="s">
+        <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="14" t="s">
+    <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="G17" s="14" t="s">
+      <c r="F18" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H17" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I17" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="J17" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="14" t="s">
+      <c r="H18" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I18" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="J18" s="14" t="s">
         <v>68</v>
+      </c>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N18">
-    <sortCondition ref="C2:C18"/>
-    <sortCondition ref="D2:D18"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y19">
+    <sortCondition ref="C2:C19"/>
+    <sortCondition ref="D2:D19"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>